<commit_message>
the new xlsx file
</commit_message>
<xml_diff>
--- a/descriptives_and_supplements.xlsx
+++ b/descriptives_and_supplements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yikaizhou/Desktop/JQL二修/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBAF3F3-7065-234F-8E99-04664413CBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2003D50-7190-4740-933E-B568862B393E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="3840" windowWidth="21600" windowHeight="18880" xr2:uid="{74BE0930-D8B9-2141-9897-BB13391439AD}"/>
+    <workbookView xWindow="-20920" yWindow="-10480" windowWidth="19700" windowHeight="18260" xr2:uid="{74BE0930-D8B9-2141-9897-BB13391439AD}"/>
   </bookViews>
   <sheets>
     <sheet name="lexical-level metrics" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
   <si>
     <t>STTR</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -59,38 +59,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">2019 iPhone introduction </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2020 iPhone introduction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2021 iPhone introduction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2022 iPhone introduction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019 Watch introduction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2020 Watch introduction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2021 Watch introduction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2022 Watch introduction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>2016 launch event</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -119,14 +87,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">2018 iPhone introduction </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2018 Watch introduction</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Mean</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -222,10 +182,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">launch mode </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>onsite</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -235,6 +191,54 @@
   </si>
   <si>
     <t>Launch mode</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Launch Mode </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tokens</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019 iPhone introduction (iPhone 11)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">2018 iPhone introduction (iPhone XS) </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020 iPhone introduction (iPhone 12)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021 iPhone introduction (iPhone 13)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022 iPhone introduction (iPhone 14)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018 Watch introduction (Watch S4)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019 Watch introduction (Watch S5)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020 Watch introduction (Watch S6)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2021 Watch introduction (Watch S7)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022 Watch introduction (Watch S8)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -357,7 +361,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -412,11 +416,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -733,19 +743,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4932993-9060-D945-9A78-77BDBBC8E072}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="38.1640625" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -762,12 +772,15 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>39</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1">
         <v>0.39600000000000002</v>
@@ -782,12 +795,15 @@
         <v>8.4480000000000004</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>36</v>
+      </c>
+      <c r="G2" s="1">
+        <v>7111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1">
         <v>0.39600000000000002</v>
@@ -802,12 +818,15 @@
         <v>8.4139999999999997</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>36</v>
+      </c>
+      <c r="G3" s="21">
+        <v>5979</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1">
         <v>0.442</v>
@@ -822,12 +841,15 @@
         <v>8.7159999999999993</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="G4" s="21">
+        <v>6771</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1">
         <v>0.45700000000000002</v>
@@ -842,12 +864,15 @@
         <v>8.5190000000000001</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="G5" s="21">
+        <v>4427</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1">
         <v>0.44900000000000001</v>
@@ -862,12 +887,15 @@
         <v>8.6120000000000001</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="G6" s="21">
+        <v>5408</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
         <v>0.42799999999999999</v>
@@ -882,10 +910,11 @@
         <v>8.5419999999999998</v>
       </c>
       <c r="F7" s="17"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>0.03</v>
@@ -900,10 +929,11 @@
         <v>0.123</v>
       </c>
       <c r="F8" s="17"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="6" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1">
         <v>0.44</v>
@@ -918,12 +948,15 @@
         <v>8.2110000000000003</v>
       </c>
       <c r="F9" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9">
+        <v>3039</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="6" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>0.42899999999999999</v>
@@ -938,12 +971,15 @@
         <v>8.2309999999999999</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>36</v>
+      </c>
+      <c r="G10">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="6" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1">
         <v>0.442</v>
@@ -958,12 +994,15 @@
         <v>8.2880000000000003</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="G11">
+        <v>3308</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1">
         <v>0.44900000000000001</v>
@@ -978,12 +1017,15 @@
         <v>7.6070000000000002</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="G12">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1">
         <v>0.46700000000000003</v>
@@ -998,12 +1040,15 @@
         <v>8.6050000000000004</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="G13">
+        <v>4553</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="7" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
         <v>0.44500000000000001</v>
@@ -1018,10 +1063,11 @@
         <v>8.1890000000000001</v>
       </c>
       <c r="F14" s="17"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="8" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1">
         <v>1.4E-2</v>
@@ -1036,10 +1082,11 @@
         <v>0.36199999999999999</v>
       </c>
       <c r="F15" s="17"/>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="9" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1">
         <v>0.40500000000000003</v>
@@ -1054,12 +1101,15 @@
         <v>8.6150000000000002</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>36</v>
+      </c>
+      <c r="G16" s="1">
+        <v>8999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1">
         <v>0.38800000000000001</v>
@@ -1074,12 +1124,15 @@
         <v>8.7420000000000009</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>36</v>
+      </c>
+      <c r="G17" s="1">
+        <v>15066</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="9" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B18" s="1">
         <v>0.40300000000000002</v>
@@ -1094,12 +1147,16 @@
         <v>8.6760000000000002</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>36</v>
+      </c>
+      <c r="G18" s="1">
+        <v>13735</v>
+      </c>
+      <c r="L18" s="18"/>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B19" s="1">
         <v>0.39800000000000002</v>
@@ -1114,12 +1171,16 @@
         <v>8.7880000000000003</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>36</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1650</v>
+      </c>
+      <c r="L19" s="18"/>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="B20" s="1">
         <v>0.441</v>
@@ -1134,12 +1195,16 @@
         <v>8.8109999999999999</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="G20" s="1">
+        <v>9024</v>
+      </c>
+      <c r="L20" s="18"/>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="9" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1">
         <v>0.45</v>
@@ -1154,12 +1219,15 @@
         <v>8.7620000000000005</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="G21" s="1">
+        <v>9246</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="9" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B22" s="1">
         <v>0.45200000000000001</v>
@@ -1174,12 +1242,15 @@
         <v>8.9979999999999993</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>37</v>
+      </c>
+      <c r="G22" s="1">
+        <v>12369</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="10" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B23" s="1">
         <v>0.42</v>
@@ -1194,10 +1265,11 @@
         <v>8.77</v>
       </c>
       <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="11" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1">
         <v>2.7E-2</v>
@@ -1212,6 +1284,7 @@
         <v>0.121</v>
       </c>
       <c r="F24" s="14"/>
+      <c r="G24" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1234,36 +1307,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="B1" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="B1" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1682,7 +1755,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1">
         <v>12.417</v>
@@ -1705,39 +1778,39 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="19">
+        <v>23</v>
+      </c>
+      <c r="B22" s="20">
         <f>STDEV(B21:G21)</f>
         <v>0.45739333911488772</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1766,74 +1839,74 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>